<commit_message>
Finished sample monthly data.
</commit_message>
<xml_diff>
--- a/heatpump/data/sample_monthly.xlsx
+++ b/heatpump/data/sample_monthly.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabb9\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17385" windowHeight="11070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17388" windowHeight="11076"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>month</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t>co2_lbs_saved</t>
-  </si>
-  <si>
-    <t>db_temp</t>
-  </si>
-  <si>
-    <t>days</t>
   </si>
 </sst>
 </file>
@@ -95,7 +89,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -143,7 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -151,14 +145,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -474,35 +465,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.44140625" customWidth="1"/>
+    <col min="19" max="19" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,506 +552,720 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <f>(61-U2)*350*V2*24/1000000</f>
+      <c r="B2" s="3">
         <v>15.846369000000005</v>
       </c>
-      <c r="C2" s="5">
-        <f>D2/0.135</f>
+      <c r="C2" s="4">
         <v>146.72563888888891</v>
       </c>
-      <c r="D2" s="5">
-        <f>B2/0.8</f>
+      <c r="D2" s="4">
         <v>19.807961250000005</v>
       </c>
-      <c r="E2" s="6">
-        <f>C2*5.2</f>
+      <c r="E2" s="5">
+        <v>762.97332222222235</v>
+      </c>
+      <c r="F2" s="4">
+        <v>146.72563888888891</v>
+      </c>
+      <c r="G2" s="3">
+        <v>19.807961250000005</v>
+      </c>
+      <c r="H2" s="5">
         <v>762.97332222222235</v>
       </c>
       <c r="I2">
         <v>450</v>
       </c>
       <c r="J2">
-        <f>0.21*I2</f>
         <v>94.5</v>
       </c>
       <c r="K2">
         <v>450</v>
       </c>
+      <c r="L2" s="7">
+        <v>94.5</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
       <c r="R2">
         <v>1.8</v>
       </c>
-      <c r="U2" s="4">
-        <v>0.14604838709677079</v>
-      </c>
-      <c r="V2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <f t="shared" ref="B3:B13" si="0">(61-U3)*350*V3*24/1000000</f>
+      <c r="B3" s="3">
         <v>14.096859</v>
       </c>
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C13" si="1">D3/0.135</f>
+      <c r="C3" s="4">
         <v>130.52647222222222</v>
       </c>
-      <c r="D3" s="5">
-        <f t="shared" ref="D3:D13" si="2">B3/0.8</f>
+      <c r="D3" s="4">
         <v>17.621073750000001</v>
       </c>
-      <c r="E3" s="6">
-        <f t="shared" ref="E3:E13" si="3">C3*5.2</f>
+      <c r="E3" s="5">
+        <v>678.73765555555565</v>
+      </c>
+      <c r="F3" s="4">
+        <v>130.52647222222222</v>
+      </c>
+      <c r="G3" s="3">
+        <v>17.621073750000001</v>
+      </c>
+      <c r="H3" s="5">
         <v>678.73765555555565</v>
       </c>
       <c r="I3">
         <v>430</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J13" si="4">0.21*I3</f>
         <v>90.3</v>
       </c>
       <c r="K3">
         <v>430</v>
       </c>
+      <c r="L3" s="7">
+        <v>90.3</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
       <c r="R3">
         <v>1.85</v>
       </c>
-      <c r="U3" s="4">
-        <v>1.064374999999997</v>
-      </c>
-      <c r="V3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <f t="shared" si="0"/>
+      <c r="B4" s="3">
         <v>15.259209</v>
       </c>
-      <c r="C4" s="5">
-        <f t="shared" si="1"/>
+      <c r="C4" s="4">
         <v>141.28897222222218</v>
       </c>
-      <c r="D4" s="5">
-        <f t="shared" si="2"/>
+      <c r="D4" s="4">
         <v>19.074011249999998</v>
       </c>
-      <c r="E4" s="6">
-        <f t="shared" si="3"/>
+      <c r="E4" s="5">
+        <v>734.70265555555534</v>
+      </c>
+      <c r="F4" s="4">
+        <v>141.28897222222218</v>
+      </c>
+      <c r="G4" s="3">
+        <v>19.074011249999998</v>
+      </c>
+      <c r="H4" s="5">
         <v>734.70265555555534</v>
       </c>
       <c r="I4">
         <v>410</v>
       </c>
       <c r="J4">
-        <f t="shared" si="4"/>
         <v>86.1</v>
       </c>
       <c r="K4">
         <v>410</v>
       </c>
+      <c r="L4" s="7">
+        <v>86.1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
       <c r="R4">
         <v>1.9</v>
       </c>
-      <c r="U4" s="4">
-        <v>2.400887096774194</v>
-      </c>
-      <c r="V4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <f t="shared" si="0"/>
+      <c r="B5" s="3">
         <v>12.243798000000005</v>
       </c>
-      <c r="C5" s="5">
-        <f t="shared" si="1"/>
+      <c r="C5" s="4">
         <v>113.36850000000004</v>
       </c>
-      <c r="D5" s="5">
-        <f t="shared" si="2"/>
+      <c r="D5" s="4">
         <v>15.304747500000007</v>
       </c>
-      <c r="E5" s="6">
-        <f t="shared" si="3"/>
+      <c r="E5" s="5">
         <v>589.51620000000025</v>
+      </c>
+      <c r="F5" s="4">
+        <v>32.391000000000005</v>
+      </c>
+      <c r="G5" s="3">
+        <v>4.3727850000000013</v>
+      </c>
+      <c r="H5" s="5">
+        <v>168.43320000000003</v>
       </c>
       <c r="I5">
         <v>390</v>
       </c>
       <c r="J5">
-        <f t="shared" si="4"/>
         <v>81.899999999999991</v>
       </c>
-      <c r="K5" s="7">
-        <f>(61-U5)*250*V5*24/3412/R5+I5</f>
+      <c r="K5" s="6">
         <v>1555.0817968666743</v>
+      </c>
+      <c r="L5" s="7">
+        <v>579.78680859000337</v>
+      </c>
+      <c r="M5" s="4">
+        <v>-80.977500000000035</v>
+      </c>
+      <c r="N5" s="4">
+        <v>-10.931962500000004</v>
+      </c>
+      <c r="O5" s="5">
+        <v>-421.0830000000002</v>
+      </c>
+      <c r="P5" s="7">
+        <v>1165.0817968666743</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>497.8868085900034</v>
       </c>
       <c r="R5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="U5" s="4">
-        <v>12.41349999999998</v>
-      </c>
-      <c r="V5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S5" s="4">
+        <v>-115.73573045534499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
+      <c r="B6" s="3">
         <v>7.923930000000003</v>
       </c>
-      <c r="C6" s="5">
-        <f t="shared" si="1"/>
+      <c r="C6" s="4">
         <v>73.369722222222251</v>
       </c>
-      <c r="D6" s="5">
-        <f t="shared" si="2"/>
+      <c r="D6" s="4">
         <v>9.9049125000000036</v>
       </c>
-      <c r="E6" s="6">
-        <f t="shared" si="3"/>
+      <c r="E6" s="5">
         <v>381.5225555555557</v>
+      </c>
+      <c r="F6" s="4">
+        <v>20.962777777777784</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2.829975000000001</v>
+      </c>
+      <c r="H6" s="5">
+        <v>109.00644444444448</v>
       </c>
       <c r="I6">
         <v>370</v>
       </c>
       <c r="J6">
-        <f t="shared" si="4"/>
         <v>77.7</v>
       </c>
-      <c r="K6" s="7">
-        <f t="shared" ref="K6:K12" si="5">(61-U6)*250*V6*24/3412/R6+I6</f>
+      <c r="K6" s="6">
         <v>888.3863936107856</v>
+      </c>
+      <c r="L6" s="7">
+        <v>279.77387712485353</v>
+      </c>
+      <c r="M6" s="4">
+        <v>-52.406944444444463</v>
+      </c>
+      <c r="N6" s="4">
+        <v>-7.0749375000000025</v>
+      </c>
+      <c r="O6" s="5">
+        <v>-272.51611111111123</v>
+      </c>
+      <c r="P6" s="7">
+        <v>518.3863936107856</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>202.07387712485354</v>
       </c>
       <c r="R6">
         <v>3.2</v>
       </c>
-      <c r="U6" s="4">
-        <v>30.57016129032257</v>
-      </c>
-      <c r="V6">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S6" s="4">
+        <v>304.46284378663563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
+      <c r="B7" s="3">
         <v>4.2073920000000031</v>
       </c>
-      <c r="C7" s="5">
-        <f t="shared" si="1"/>
+      <c r="C7" s="4">
         <v>38.957333333333359</v>
       </c>
-      <c r="D7" s="5">
-        <f t="shared" si="2"/>
+      <c r="D7" s="4">
         <v>5.2592400000000037</v>
       </c>
-      <c r="E7" s="6">
-        <f t="shared" si="3"/>
+      <c r="E7" s="5">
         <v>202.57813333333348</v>
+      </c>
+      <c r="F7" s="4">
+        <v>11.130666666666682</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.5026400000000022</v>
+      </c>
+      <c r="H7" s="5">
+        <v>57.879466666666751</v>
       </c>
       <c r="I7">
         <v>350</v>
       </c>
       <c r="J7">
-        <f t="shared" si="4"/>
         <v>73.5</v>
       </c>
-      <c r="K7" s="7">
-        <f t="shared" si="5"/>
+      <c r="K7" s="6">
         <v>601.65633897169664</v>
+      </c>
+      <c r="L7" s="7">
+        <v>150.7453525372635</v>
+      </c>
+      <c r="M7" s="4">
+        <v>-27.826666666666675</v>
+      </c>
+      <c r="N7" s="4">
+        <v>-3.7566000000000015</v>
+      </c>
+      <c r="O7" s="5">
+        <v>-144.69866666666672</v>
+      </c>
+      <c r="P7" s="7">
+        <v>251.65633897169664</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>77.2453525372635</v>
       </c>
       <c r="R7">
         <v>3.5</v>
       </c>
-      <c r="U7" s="4">
-        <v>44.303999999999988</v>
-      </c>
-      <c r="V7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S7" s="4">
+        <v>199.64589425556858</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
+      <c r="B8" s="3">
         <v>1.4398440000000172</v>
       </c>
-      <c r="C8" s="5">
-        <f t="shared" si="1"/>
+      <c r="C8" s="4">
         <v>13.331888888889047</v>
       </c>
-      <c r="D8" s="5">
-        <f t="shared" si="2"/>
+      <c r="D8" s="4">
         <v>1.7998050000000214</v>
       </c>
-      <c r="E8" s="6">
-        <f t="shared" si="3"/>
+      <c r="E8" s="5">
         <v>69.325822222223053</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.80911111111116</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.51423000000000663</v>
+      </c>
+      <c r="H8" s="5">
+        <v>19.807377777778033</v>
       </c>
       <c r="I8">
         <v>370</v>
       </c>
       <c r="J8">
-        <f t="shared" si="4"/>
         <v>77.7</v>
       </c>
-      <c r="K8" s="7">
-        <f t="shared" si="5"/>
+      <c r="K8" s="6">
         <v>456.12125272148819</v>
+      </c>
+      <c r="L8" s="7">
+        <v>95.78546307151251</v>
+      </c>
+      <c r="M8" s="4">
+        <v>-9.5227777777778861</v>
+      </c>
+      <c r="N8" s="4">
+        <v>-1.2855750000000148</v>
+      </c>
+      <c r="O8" s="5">
+        <v>-49.518444444445024</v>
+      </c>
+      <c r="P8" s="7">
+        <v>86.12125272148819</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>18.085463071512507</v>
       </c>
       <c r="R8">
         <v>3.5</v>
       </c>
-      <c r="U8" s="4">
-        <v>55.470645161290257</v>
-      </c>
-      <c r="V8">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S8" s="4">
+        <v>68.322358118406385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
+      <c r="B9" s="3">
         <v>2.0285159999999629</v>
       </c>
-      <c r="C9" s="5">
-        <f t="shared" si="1"/>
+      <c r="C9" s="4">
         <v>18.782555555555209</v>
       </c>
-      <c r="D9" s="5">
-        <f t="shared" si="2"/>
+      <c r="D9" s="4">
         <v>2.5356449999999535</v>
       </c>
-      <c r="E9" s="6">
-        <f t="shared" si="3"/>
+      <c r="E9" s="5">
         <v>97.669288888887095</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5.3664444444443458</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.72446999999998674</v>
+      </c>
+      <c r="H9" s="5">
+        <v>27.905511111110599</v>
       </c>
       <c r="I9">
         <v>390</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
         <v>81.899999999999991</v>
       </c>
-      <c r="K9" s="7">
-        <f t="shared" si="5"/>
+      <c r="K9" s="6">
         <v>511.33143527047173</v>
+      </c>
+      <c r="L9" s="7">
+        <v>110.09914587171228</v>
+      </c>
+      <c r="M9" s="4">
+        <v>-13.416111111110864</v>
+      </c>
+      <c r="N9" s="4">
+        <v>-1.8111749999999667</v>
+      </c>
+      <c r="O9" s="5">
+        <v>-69.763777777776497</v>
+      </c>
+      <c r="P9" s="7">
+        <v>121.33143527047173</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>28.19914587171229</v>
       </c>
       <c r="R9">
         <v>3.5</v>
       </c>
-      <c r="U9" s="4">
-        <v>53.210000000000143</v>
-      </c>
-      <c r="V9">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S9" s="4">
+        <v>96.255564214535156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
+      <c r="B10" s="3">
         <v>4.4438939999999922</v>
       </c>
-      <c r="C10" s="5">
-        <f t="shared" si="1"/>
+      <c r="C10" s="4">
         <v>41.147166666666585</v>
       </c>
-      <c r="D10" s="5">
-        <f t="shared" si="2"/>
+      <c r="D10" s="4">
         <v>5.5548674999999896</v>
       </c>
-      <c r="E10" s="6">
-        <f t="shared" si="3"/>
+      <c r="E10" s="5">
         <v>213.96526666666625</v>
+      </c>
+      <c r="F10" s="4">
+        <v>11.756333333333314</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.5871049999999975</v>
+      </c>
+      <c r="H10" s="5">
+        <v>61.132933333333234</v>
       </c>
       <c r="I10">
         <v>410</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
         <v>86.1</v>
       </c>
-      <c r="K10" s="7">
-        <f t="shared" si="5"/>
+      <c r="K10" s="6">
         <v>675.8022106849769</v>
+      </c>
+      <c r="L10" s="7">
+        <v>184.11099480823961</v>
+      </c>
+      <c r="M10" s="4">
+        <v>-29.390833333333269</v>
+      </c>
+      <c r="N10" s="4">
+        <v>-3.9677624999999921</v>
+      </c>
+      <c r="O10" s="5">
+        <v>-152.83233333333303</v>
+      </c>
+      <c r="P10" s="7">
+        <v>265.8022106849769</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>98.010994808239616</v>
       </c>
       <c r="R10">
         <v>3.5</v>
       </c>
-      <c r="U10" s="4">
-        <v>43.365500000000033</v>
-      </c>
-      <c r="V10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S10" s="4">
+        <v>210.86820329718586</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
+      <c r="B11" s="3">
         <v>9.4632719999999964</v>
       </c>
-      <c r="C11" s="5">
-        <f t="shared" si="1"/>
+      <c r="C11" s="4">
         <v>87.622888888888852</v>
       </c>
-      <c r="D11" s="5">
-        <f t="shared" si="2"/>
+      <c r="D11" s="4">
         <v>11.829089999999995</v>
       </c>
-      <c r="E11" s="6">
-        <f t="shared" si="3"/>
+      <c r="E11" s="5">
         <v>455.63902222222202</v>
+      </c>
+      <c r="F11" s="4">
+        <v>25.035111111111075</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.3797399999999955</v>
+      </c>
+      <c r="H11" s="5">
+        <v>130.1825777777776</v>
       </c>
       <c r="I11">
         <v>430</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
         <v>90.3</v>
       </c>
-      <c r="K11" s="7">
-        <f t="shared" si="5"/>
+      <c r="K11" s="6">
         <v>1090.3634232121922</v>
+      </c>
+      <c r="L11" s="7">
+        <v>370.66354044548649</v>
+      </c>
+      <c r="M11" s="4">
+        <v>-62.587777777777774</v>
+      </c>
+      <c r="N11" s="4">
+        <v>-8.449349999999999</v>
+      </c>
+      <c r="O11" s="5">
+        <v>-325.4564444444444</v>
+      </c>
+      <c r="P11" s="7">
+        <v>660.36342321219217</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>280.36354044548648</v>
       </c>
       <c r="R11">
         <v>3</v>
       </c>
-      <c r="U11" s="4">
-        <v>24.65870967741937</v>
-      </c>
-      <c r="V11">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S11" s="4">
+        <v>297.16023862837028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
-        <f t="shared" si="0"/>
+      <c r="B12" s="3">
         <v>13.032873</v>
       </c>
-      <c r="C12" s="5">
-        <f t="shared" si="1"/>
+      <c r="C12" s="4">
         <v>120.67475</v>
       </c>
-      <c r="D12" s="5">
-        <f t="shared" si="2"/>
+      <c r="D12" s="4">
         <v>16.291091250000001</v>
       </c>
-      <c r="E12" s="6">
-        <f t="shared" si="3"/>
+      <c r="E12" s="5">
         <v>627.50870000000009</v>
+      </c>
+      <c r="F12" s="4">
+        <v>34.478500000000004</v>
+      </c>
+      <c r="G12" s="3">
+        <v>4.6545975000000013</v>
+      </c>
+      <c r="H12" s="5">
+        <v>179.28820000000002</v>
       </c>
       <c r="I12">
         <v>430</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
         <v>90.3</v>
       </c>
-      <c r="K12" s="7">
-        <f t="shared" si="5"/>
+      <c r="K12" s="6">
         <v>1670.1677235425768</v>
+      </c>
+      <c r="L12" s="7">
+        <v>631.57547559415957</v>
+      </c>
+      <c r="M12" s="4">
+        <v>-86.196249999999992</v>
+      </c>
+      <c r="N12" s="4">
+        <v>-11.63649375</v>
+      </c>
+      <c r="O12" s="5">
+        <v>-448.22050000000007</v>
+      </c>
+      <c r="P12" s="7">
+        <v>1240.1677235425768</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>541.27547559415962</v>
       </c>
       <c r="R12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="U12" s="4">
-        <v>9.2822499999999959</v>
-      </c>
-      <c r="V12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S12" s="4">
+        <v>-123.19454115354893</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
-        <f t="shared" si="0"/>
+      <c r="B13" s="3">
         <v>15.590337</v>
       </c>
-      <c r="C13" s="5">
-        <f t="shared" si="1"/>
+      <c r="C13" s="4">
         <v>144.35497222222222</v>
       </c>
-      <c r="D13" s="5">
-        <f t="shared" si="2"/>
+      <c r="D13" s="4">
         <v>19.487921249999999</v>
       </c>
-      <c r="E13" s="6">
-        <f t="shared" si="3"/>
+      <c r="E13" s="5">
+        <v>750.6458555555555</v>
+      </c>
+      <c r="F13" s="4">
+        <v>144.35497222222222</v>
+      </c>
+      <c r="G13" s="3">
+        <v>19.487921249999999</v>
+      </c>
+      <c r="H13" s="5">
         <v>750.6458555555555</v>
       </c>
       <c r="I13">
         <v>450</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
         <v>94.5</v>
       </c>
       <c r="K13">
         <v>450</v>
       </c>
+      <c r="L13" s="7">
+        <v>94.5</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
       <c r="R13">
         <v>1.85</v>
       </c>
-      <c r="U13" s="4">
-        <v>1.129274193548387</v>
-      </c>
-      <c r="V13">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K15" s="6"/>
+      <c r="S13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added cash flow and financial sample data to heat pump model.
</commit_message>
<xml_diff>
--- a/heatpump/data/sample_monthly.xlsx
+++ b/heatpump/data/sample_monthly.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabb9\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\heat-pump-calc\heatpump\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17388" windowHeight="11076"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17385" windowHeight="11070"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="with_pce" sheetId="1" r:id="rId1"/>
+    <sheet name="without_pce" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>month</t>
   </si>
@@ -38,28 +39,16 @@
     <t>fuel_mmbtu_no_hp</t>
   </si>
   <si>
-    <t>fuel_$_no_hp</t>
-  </si>
-  <si>
     <t>fuel_units_w_hp</t>
   </si>
   <si>
     <t>fuel_mmbtu_w_hp</t>
   </si>
   <si>
-    <t>fuel_$_w_hp</t>
-  </si>
-  <si>
     <t>elec_kwh_no_hp</t>
   </si>
   <si>
-    <t>elec_$_no_hp</t>
-  </si>
-  <si>
     <t>elec_kwh_w_hp</t>
-  </si>
-  <si>
-    <t>elec_$_w_hp</t>
   </si>
   <si>
     <t>fuel_chg_units</t>
@@ -68,13 +57,7 @@
     <t>fuel_chg_mmbtu</t>
   </si>
   <si>
-    <t>fuel_chg_$</t>
-  </si>
-  <si>
     <t>elec_chg_kwh</t>
-  </si>
-  <si>
-    <t>elec_chg_$</t>
   </si>
   <si>
     <t>cop</t>
@@ -82,14 +65,33 @@
   <si>
     <t>co2_lbs_saved</t>
   </si>
+  <si>
+    <t>fuel_dol_no_hp</t>
+  </si>
+  <si>
+    <t>fuel_dol_w_hp</t>
+  </si>
+  <si>
+    <t>elec_dol_no_hp</t>
+  </si>
+  <si>
+    <t>elec_dol_w_hp</t>
+  </si>
+  <si>
+    <t>fuel_chg_dol</t>
+  </si>
+  <si>
+    <t>elec_chg_dol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -137,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,6 +152,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -468,33 +471,33 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.44140625" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -508,52 +511,52 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -671,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -730,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -789,7 +792,7 @@
         <v>-115.73573045534499</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -848,7 +851,7 @@
         <v>304.46284378663563</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -907,7 +910,7 @@
         <v>199.64589425556858</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -966,7 +969,7 @@
         <v>68.322358118406385</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>96.255564214535156</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>210.86820329718586</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>297.16023862837028</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>-123.19454115354893</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1261,10 +1264,819 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection sqref="A1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>15.846369000000005</v>
+      </c>
+      <c r="C2" s="4">
+        <v>146.72563888888891</v>
+      </c>
+      <c r="D2" s="4">
+        <v>19.807961250000005</v>
+      </c>
+      <c r="E2" s="5">
+        <v>762.97332222222235</v>
+      </c>
+      <c r="F2" s="4">
+        <v>146.72563888888891</v>
+      </c>
+      <c r="G2" s="3">
+        <v>19.807961250000005</v>
+      </c>
+      <c r="H2" s="5">
+        <v>762.97332222222235</v>
+      </c>
+      <c r="I2">
+        <v>450</v>
+      </c>
+      <c r="J2">
+        <v>202.5</v>
+      </c>
+      <c r="K2">
+        <v>450</v>
+      </c>
+      <c r="L2" s="8">
+        <v>202.5</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1.8</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>14.096859</v>
+      </c>
+      <c r="C3" s="4">
+        <v>130.52647222222222</v>
+      </c>
+      <c r="D3" s="4">
+        <v>17.621073750000001</v>
+      </c>
+      <c r="E3" s="5">
+        <v>678.73765555555565</v>
+      </c>
+      <c r="F3" s="4">
+        <v>130.52647222222222</v>
+      </c>
+      <c r="G3" s="3">
+        <v>17.621073750000001</v>
+      </c>
+      <c r="H3" s="5">
+        <v>678.73765555555565</v>
+      </c>
+      <c r="I3">
+        <v>430</v>
+      </c>
+      <c r="J3">
+        <v>193.5</v>
+      </c>
+      <c r="K3">
+        <v>430</v>
+      </c>
+      <c r="L3" s="8">
+        <v>193.5</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1.85</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>15.259209</v>
+      </c>
+      <c r="C4" s="4">
+        <v>141.28897222222218</v>
+      </c>
+      <c r="D4" s="4">
+        <v>19.074011249999998</v>
+      </c>
+      <c r="E4" s="5">
+        <v>734.70265555555534</v>
+      </c>
+      <c r="F4" s="4">
+        <v>141.28897222222218</v>
+      </c>
+      <c r="G4" s="3">
+        <v>19.074011249999998</v>
+      </c>
+      <c r="H4" s="5">
+        <v>734.70265555555534</v>
+      </c>
+      <c r="I4">
+        <v>410</v>
+      </c>
+      <c r="J4">
+        <v>184.5</v>
+      </c>
+      <c r="K4">
+        <v>410</v>
+      </c>
+      <c r="L4" s="8">
+        <v>184.5</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1.9</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12.243798000000005</v>
+      </c>
+      <c r="C5" s="4">
+        <v>113.36850000000004</v>
+      </c>
+      <c r="D5" s="4">
+        <v>15.304747500000007</v>
+      </c>
+      <c r="E5" s="5">
+        <v>589.51620000000025</v>
+      </c>
+      <c r="F5" s="4">
+        <v>32.391000000000005</v>
+      </c>
+      <c r="G5" s="3">
+        <v>4.3727850000000013</v>
+      </c>
+      <c r="H5" s="5">
+        <v>168.43320000000003</v>
+      </c>
+      <c r="I5">
+        <v>390</v>
+      </c>
+      <c r="J5">
+        <v>175.5</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1555.0817968666743</v>
+      </c>
+      <c r="L5" s="8">
+        <v>699.78680859000349</v>
+      </c>
+      <c r="M5" s="4">
+        <v>-80.977500000000035</v>
+      </c>
+      <c r="N5" s="4">
+        <v>-10.931962500000004</v>
+      </c>
+      <c r="O5" s="5">
+        <v>-421.0830000000002</v>
+      </c>
+      <c r="P5" s="7">
+        <v>1165.0817968666743</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>524.28680859000349</v>
+      </c>
+      <c r="R5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S5" s="4">
+        <v>-115.73573045534499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>7.923930000000003</v>
+      </c>
+      <c r="C6" s="4">
+        <v>73.369722222222251</v>
+      </c>
+      <c r="D6" s="4">
+        <v>9.9049125000000036</v>
+      </c>
+      <c r="E6" s="5">
+        <v>381.5225555555557</v>
+      </c>
+      <c r="F6" s="4">
+        <v>20.962777777777784</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2.829975000000001</v>
+      </c>
+      <c r="H6" s="5">
+        <v>109.00644444444448</v>
+      </c>
+      <c r="I6">
+        <v>370</v>
+      </c>
+      <c r="J6">
+        <v>166.5</v>
+      </c>
+      <c r="K6" s="6">
+        <v>888.3863936107856</v>
+      </c>
+      <c r="L6" s="8">
+        <v>399.77387712485353</v>
+      </c>
+      <c r="M6" s="4">
+        <v>-52.406944444444463</v>
+      </c>
+      <c r="N6" s="4">
+        <v>-7.0749375000000025</v>
+      </c>
+      <c r="O6" s="5">
+        <v>-272.51611111111123</v>
+      </c>
+      <c r="P6" s="7">
+        <v>518.3863936107856</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>233.27387712485353</v>
+      </c>
+      <c r="R6">
+        <v>3.2</v>
+      </c>
+      <c r="S6" s="4">
+        <v>304.46284378663563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4.2073920000000031</v>
+      </c>
+      <c r="C7" s="4">
+        <v>38.957333333333359</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5.2592400000000037</v>
+      </c>
+      <c r="E7" s="5">
+        <v>202.57813333333348</v>
+      </c>
+      <c r="F7" s="4">
+        <v>11.130666666666682</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.5026400000000022</v>
+      </c>
+      <c r="H7" s="5">
+        <v>57.879466666666751</v>
+      </c>
+      <c r="I7">
+        <v>350</v>
+      </c>
+      <c r="J7">
+        <v>157.5</v>
+      </c>
+      <c r="K7" s="6">
+        <v>601.65633897169664</v>
+      </c>
+      <c r="L7" s="8">
+        <v>270.7453525372635</v>
+      </c>
+      <c r="M7" s="4">
+        <v>-27.826666666666675</v>
+      </c>
+      <c r="N7" s="4">
+        <v>-3.7566000000000015</v>
+      </c>
+      <c r="O7" s="5">
+        <v>-144.69866666666672</v>
+      </c>
+      <c r="P7" s="7">
+        <v>251.65633897169664</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>113.2453525372635</v>
+      </c>
+      <c r="R7">
+        <v>3.5</v>
+      </c>
+      <c r="S7" s="4">
+        <v>199.64589425556858</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.4398440000000172</v>
+      </c>
+      <c r="C8" s="4">
+        <v>13.331888888889047</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.7998050000000214</v>
+      </c>
+      <c r="E8" s="5">
+        <v>69.325822222223053</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.80911111111116</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.51423000000000663</v>
+      </c>
+      <c r="H8" s="5">
+        <v>19.807377777778033</v>
+      </c>
+      <c r="I8">
+        <v>370</v>
+      </c>
+      <c r="J8">
+        <v>166.5</v>
+      </c>
+      <c r="K8" s="6">
+        <v>456.12125272148819</v>
+      </c>
+      <c r="L8" s="8">
+        <v>205.25456372466968</v>
+      </c>
+      <c r="M8" s="4">
+        <v>-9.5227777777778861</v>
+      </c>
+      <c r="N8" s="4">
+        <v>-1.2855750000000148</v>
+      </c>
+      <c r="O8" s="5">
+        <v>-49.518444444445024</v>
+      </c>
+      <c r="P8" s="7">
+        <v>86.12125272148819</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>38.75456372466968</v>
+      </c>
+      <c r="R8">
+        <v>3.5</v>
+      </c>
+      <c r="S8" s="4">
+        <v>68.322358118406385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.0285159999999629</v>
+      </c>
+      <c r="C9" s="4">
+        <v>18.782555555555209</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.5356449999999535</v>
+      </c>
+      <c r="E9" s="5">
+        <v>97.669288888887095</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5.3664444444443458</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.72446999999998674</v>
+      </c>
+      <c r="H9" s="5">
+        <v>27.905511111110599</v>
+      </c>
+      <c r="I9">
+        <v>390</v>
+      </c>
+      <c r="J9">
+        <v>175.5</v>
+      </c>
+      <c r="K9" s="6">
+        <v>511.33143527047173</v>
+      </c>
+      <c r="L9" s="8">
+        <v>230.0991458717123</v>
+      </c>
+      <c r="M9" s="4">
+        <v>-13.416111111110864</v>
+      </c>
+      <c r="N9" s="4">
+        <v>-1.8111749999999667</v>
+      </c>
+      <c r="O9" s="5">
+        <v>-69.763777777776497</v>
+      </c>
+      <c r="P9" s="7">
+        <v>121.33143527047173</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>54.599145871712295</v>
+      </c>
+      <c r="R9">
+        <v>3.5</v>
+      </c>
+      <c r="S9" s="4">
+        <v>96.255564214535156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4.4438939999999922</v>
+      </c>
+      <c r="C10" s="4">
+        <v>41.147166666666585</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5.5548674999999896</v>
+      </c>
+      <c r="E10" s="5">
+        <v>213.96526666666625</v>
+      </c>
+      <c r="F10" s="4">
+        <v>11.756333333333314</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.5871049999999975</v>
+      </c>
+      <c r="H10" s="5">
+        <v>61.132933333333234</v>
+      </c>
+      <c r="I10">
+        <v>410</v>
+      </c>
+      <c r="J10">
+        <v>184.5</v>
+      </c>
+      <c r="K10" s="6">
+        <v>675.8022106849769</v>
+      </c>
+      <c r="L10" s="8">
+        <v>304.11099480823964</v>
+      </c>
+      <c r="M10" s="4">
+        <v>-29.390833333333269</v>
+      </c>
+      <c r="N10" s="4">
+        <v>-3.9677624999999921</v>
+      </c>
+      <c r="O10" s="5">
+        <v>-152.83233333333303</v>
+      </c>
+      <c r="P10" s="7">
+        <v>265.8022106849769</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>119.61099480823964</v>
+      </c>
+      <c r="R10">
+        <v>3.5</v>
+      </c>
+      <c r="S10" s="4">
+        <v>210.86820329718586</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9.4632719999999964</v>
+      </c>
+      <c r="C11" s="4">
+        <v>87.622888888888852</v>
+      </c>
+      <c r="D11" s="4">
+        <v>11.829089999999995</v>
+      </c>
+      <c r="E11" s="5">
+        <v>455.63902222222202</v>
+      </c>
+      <c r="F11" s="4">
+        <v>25.035111111111075</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.3797399999999955</v>
+      </c>
+      <c r="H11" s="5">
+        <v>130.1825777777776</v>
+      </c>
+      <c r="I11">
+        <v>430</v>
+      </c>
+      <c r="J11">
+        <v>193.5</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1090.3634232121922</v>
+      </c>
+      <c r="L11" s="8">
+        <v>490.66354044548649</v>
+      </c>
+      <c r="M11" s="4">
+        <v>-62.587777777777774</v>
+      </c>
+      <c r="N11" s="4">
+        <v>-8.449349999999999</v>
+      </c>
+      <c r="O11" s="5">
+        <v>-325.4564444444444</v>
+      </c>
+      <c r="P11" s="7">
+        <v>660.36342321219217</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>297.16354044548649</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11" s="4">
+        <v>297.16023862837028</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>13.032873</v>
+      </c>
+      <c r="C12" s="4">
+        <v>120.67475</v>
+      </c>
+      <c r="D12" s="4">
+        <v>16.291091250000001</v>
+      </c>
+      <c r="E12" s="5">
+        <v>627.50870000000009</v>
+      </c>
+      <c r="F12" s="4">
+        <v>34.478500000000004</v>
+      </c>
+      <c r="G12" s="3">
+        <v>4.6545975000000013</v>
+      </c>
+      <c r="H12" s="5">
+        <v>179.28820000000002</v>
+      </c>
+      <c r="I12">
+        <v>430</v>
+      </c>
+      <c r="J12">
+        <v>193.5</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1670.1677235425768</v>
+      </c>
+      <c r="L12" s="8">
+        <v>751.57547559415957</v>
+      </c>
+      <c r="M12" s="4">
+        <v>-86.196249999999992</v>
+      </c>
+      <c r="N12" s="4">
+        <v>-11.63649375</v>
+      </c>
+      <c r="O12" s="5">
+        <v>-448.22050000000007</v>
+      </c>
+      <c r="P12" s="7">
+        <v>1240.1677235425768</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>558.07547559415957</v>
+      </c>
+      <c r="R12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S12" s="4">
+        <v>-123.19454115354893</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>15.590337</v>
+      </c>
+      <c r="C13" s="4">
+        <v>144.35497222222222</v>
+      </c>
+      <c r="D13" s="4">
+        <v>19.487921249999999</v>
+      </c>
+      <c r="E13" s="5">
+        <v>750.6458555555555</v>
+      </c>
+      <c r="F13" s="4">
+        <v>144.35497222222222</v>
+      </c>
+      <c r="G13" s="3">
+        <v>19.487921249999999</v>
+      </c>
+      <c r="H13" s="5">
+        <v>750.6458555555555</v>
+      </c>
+      <c r="I13">
+        <v>450</v>
+      </c>
+      <c r="J13">
+        <v>202.5</v>
+      </c>
+      <c r="K13">
+        <v>450</v>
+      </c>
+      <c r="L13" s="8">
+        <v>202.5</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1.85</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K15" s="5"/>
     </row>
   </sheetData>

</xml_diff>